<commit_message>
minor change to cd_type description
</commit_message>
<xml_diff>
--- a/template/ModelDB_template.xlsx
+++ b/template/ModelDB_template.xlsx
@@ -70,7 +70,7 @@
     <t xml:space="preserve">CD_CODE are subsets of CD_TYPE. Each term is a specific example of CD_TYPE.</t>
   </si>
   <si>
-    <t xml:space="preserve">CD_TYPE should be in all CAPS and </t>
+    <t xml:space="preserve">CD_TYPE should be in all CAPS and be a general category</t>
   </si>
   <si>
     <t xml:space="preserve">DS_DESC  is optional for a metadata term</t>
@@ -746,7 +746,7 @@
   <dimension ref="1:42"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -11046,7 +11046,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" s="4" customFormat="true" ht="46.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" s="4" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
@@ -12651,7 +12651,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
+      <selection pane="bottomLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>

<commit_message>
Added descriptions to the headers
</commit_message>
<xml_diff>
--- a/template/ModelDB_template.xlsx
+++ b/template/ModelDB_template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="118">
   <si>
     <t xml:space="preserve">ModelDB: Minimalistic Multi-Omic Data Integration</t>
   </si>
@@ -190,6 +190,9 @@
     <t xml:space="preserve">MFI_CD63_single_neutrophils</t>
   </si>
   <si>
+    <t xml:space="preserve">METADATA</t>
+  </si>
+  <si>
     <t xml:space="preserve">CD_EXPERIMENT</t>
   </si>
   <si>
@@ -248,6 +251,9 @@
   </si>
   <si>
     <t xml:space="preserve">DREAM_8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subjects may also be cell lines or genetic variants.</t>
   </si>
   <si>
     <t xml:space="preserve">CD_EXPERIMENT </t>
@@ -310,6 +316,9 @@
     <t xml:space="preserve">Each aliquot should only have one data format.</t>
   </si>
   <si>
+    <t xml:space="preserve">The source of the aliquot should be a METADATA term.</t>
+  </si>
+  <si>
     <t xml:space="preserve">CD_EXPERIMENT </t>
   </si>
   <si>
@@ -335,6 +344,9 @@
   </si>
   <si>
     <t xml:space="preserve">TISSUE_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The DATA table contains the numerical values measured.</t>
   </si>
   <si>
     <t xml:space="preserve">ID_EXPERIMENT </t>
@@ -528,7 +540,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -574,6 +586,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -745,7 +761,7 @@
   </sheetPr>
   <dimension ref="1:42"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -11289,7 +11305,7 @@
   <dimension ref="1:23"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -11303,11 +11319,17 @@
   </cols>
   <sheetData>
     <row r="1" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="8"/>
       <c r="AMJ1" s="8"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>16</v>
@@ -11339,7 +11361,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>19</v>
@@ -11371,7 +11393,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>29</v>
@@ -11385,7 +11407,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>29</v>
@@ -11399,7 +11421,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>29</v>
@@ -11413,7 +11435,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>29</v>
@@ -11427,7 +11449,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>29</v>
@@ -11444,7 +11466,7 @@
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>29</v>
@@ -11458,7 +11480,7 @@
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>29</v>
@@ -11481,15 +11503,15 @@
         <v>27</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>27</v>
@@ -11500,111 +11522,111 @@
         <v>28</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="9" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="9" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="9" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="9" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="9" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="9" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -11623,10 +11645,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A3:Q11"/>
+  <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -11636,12 +11658,23 @@
     <col collapsed="false" hidden="false" max="1025" min="3" style="11" width="8.36734693877551"/>
   </cols>
   <sheetData>
+    <row r="1" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8"/>
+      <c r="B1" s="8" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C2" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>16</v>
@@ -11691,10 +11724,10 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C4" s="11" t="s">
         <v>19</v>
@@ -11744,58 +11777,58 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B7" s="0" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>77</v>
-      </c>
       <c r="D7" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="11" t="s">
         <v>80</v>
-      </c>
-      <c r="C8" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11805,13 +11838,13 @@
       <c r="B10" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="12" t="n">
+      <c r="C10" s="13" t="n">
         <v>33137</v>
       </c>
       <c r="D10" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F10" s="12" t="n">
+      <c r="F10" s="13" t="n">
         <v>33137</v>
       </c>
       <c r="G10" s="11" t="s">
@@ -11837,13 +11870,13 @@
       <c r="B11" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C11" s="12" t="n">
+      <c r="C11" s="13" t="n">
         <v>33138</v>
       </c>
       <c r="D11" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="F11" s="12" t="n">
+      <c r="F11" s="13" t="n">
         <v>33141</v>
       </c>
       <c r="G11" s="11" t="s">
@@ -11895,30 +11928,30 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="D1" s="0" t="s">
         <v>17</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="C2" s="0" t="s">
         <v>19</v>
@@ -11930,7 +11963,7 @@
         <v>19</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11941,13 +11974,13 @@
         <v>4</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>15072</v>
@@ -11961,13 +11994,13 @@
         <v>4</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>6487</v>
@@ -11981,13 +12014,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>89</v>
-      </c>
       <c r="E6" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>13004</v>
@@ -12001,13 +12034,13 @@
         <v>4</v>
       </c>
       <c r="C7" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D7" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="D7" s="0" t="s">
-        <v>89</v>
-      </c>
       <c r="E7" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>16416</v>
@@ -12021,13 +12054,13 @@
         <v>4</v>
       </c>
       <c r="C8" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="D8" s="0" t="s">
-        <v>89</v>
-      </c>
       <c r="E8" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>8173</v>
@@ -12041,13 +12074,13 @@
         <v>4</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F9" s="0" t="n">
         <v>4312</v>
@@ -12061,13 +12094,13 @@
         <v>4</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F10" s="0" t="n">
         <v>4768</v>
@@ -12091,8 +12124,8 @@
   </sheetPr>
   <dimension ref="A1:O17"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B21" activeCellId="0" sqref="B21"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -12105,41 +12138,51 @@
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="12.6071428571429"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="11" width="12.7704081632653"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="11" width="14.1020408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="11" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="11" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="11" width="11.3571428571429"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="11" width="8.36734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" s="14" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="H1" s="14" t="s">
-        <v>93</v>
+    <row r="1" s="15" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="H1" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="K1" s="15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G2" s="11" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>16</v>
@@ -12171,22 +12214,22 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D4" s="0" t="s">
         <v>19</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="G4" s="11" t="s">
         <v>19</v>
@@ -12216,31 +12259,31 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="15"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-    </row>
-    <row r="6" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="16"/>
+      <c r="B5" s="16"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16"/>
+      <c r="F5" s="16"/>
+    </row>
+    <row r="6" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="17" t="n">
+        <v>60</v>
+      </c>
+      <c r="B6" s="18" t="n">
         <v>1</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D6" s="17" t="n">
+        <v>83</v>
+      </c>
+      <c r="D6" s="18" t="n">
         <v>100</v>
       </c>
-      <c r="E6" s="18" t="n">
+      <c r="E6" s="19" t="n">
         <v>41545</v>
       </c>
-      <c r="F6" s="17" t="n">
+      <c r="F6" s="18" t="n">
         <v>5891</v>
       </c>
       <c r="G6" s="11" t="s">
@@ -12252,30 +12295,30 @@
       <c r="I6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="K6" s="19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J6" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="K6" s="20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="17" t="n">
+        <v>60</v>
+      </c>
+      <c r="B7" s="18" t="n">
         <v>2</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="D7" s="17" t="n">
+        <v>78</v>
+      </c>
+      <c r="D7" s="18" t="n">
         <v>10062</v>
       </c>
-      <c r="E7" s="18" t="n">
+      <c r="E7" s="19" t="n">
         <v>41521</v>
       </c>
-      <c r="F7" s="17" t="n">
+      <c r="F7" s="18" t="n">
         <v>6042</v>
       </c>
       <c r="G7" s="11" t="s">
@@ -12287,30 +12330,30 @@
       <c r="I7" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J7" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="K7" s="19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="8" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J7" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="K7" s="20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="17" t="n">
+        <v>60</v>
+      </c>
+      <c r="B8" s="18" t="n">
         <v>3</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="D8" s="17" t="n">
+        <v>81</v>
+      </c>
+      <c r="D8" s="18" t="n">
         <v>10063</v>
       </c>
-      <c r="E8" s="18" t="n">
+      <c r="E8" s="19" t="n">
         <v>41521</v>
       </c>
-      <c r="F8" s="17" t="n">
+      <c r="F8" s="18" t="n">
         <v>5648</v>
       </c>
       <c r="G8" s="11" t="s">
@@ -12322,30 +12365,30 @@
       <c r="I8" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="K8" s="19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J8" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="K8" s="20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="9" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="20" t="n">
+        <v>60</v>
+      </c>
+      <c r="B9" s="21" t="n">
         <v>4</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>80</v>
-      </c>
-      <c r="D9" s="20" t="n">
+        <v>82</v>
+      </c>
+      <c r="D9" s="21" t="n">
         <v>10064</v>
       </c>
-      <c r="E9" s="21" t="n">
+      <c r="E9" s="22" t="n">
         <v>41521</v>
       </c>
-      <c r="F9" s="20" t="n">
+      <c r="F9" s="21" t="n">
         <v>3041</v>
       </c>
       <c r="G9" s="11" t="s">
@@ -12357,30 +12400,30 @@
       <c r="I9" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J9" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="K9" s="19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="10" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J9" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="K9" s="20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="10" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="17" t="n">
+        <v>60</v>
+      </c>
+      <c r="B10" s="18" t="n">
         <v>5</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D10" s="17" t="n">
+        <v>83</v>
+      </c>
+      <c r="D10" s="18" t="n">
         <v>10066</v>
       </c>
-      <c r="E10" s="18" t="n">
+      <c r="E10" s="19" t="n">
         <v>41521</v>
       </c>
-      <c r="F10" s="17" t="n">
+      <c r="F10" s="18" t="n">
         <v>6466</v>
       </c>
       <c r="G10" s="11" t="s">
@@ -12392,30 +12435,30 @@
       <c r="I10" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J10" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="K10" s="19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J10" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="K10" s="20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="11" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="17" t="n">
+        <v>60</v>
+      </c>
+      <c r="B11" s="18" t="n">
         <v>6</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D11" s="17" t="n">
+        <v>83</v>
+      </c>
+      <c r="D11" s="18" t="n">
         <v>10067</v>
       </c>
-      <c r="E11" s="18" t="n">
+      <c r="E11" s="19" t="n">
         <v>41521</v>
       </c>
-      <c r="F11" s="17"/>
+      <c r="F11" s="18"/>
       <c r="G11" s="11" t="s">
         <v>31</v>
       </c>
@@ -12425,30 +12468,30 @@
       <c r="I11" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J11" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="K11" s="19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J11" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" s="17" t="n">
+        <v>60</v>
+      </c>
+      <c r="B12" s="18" t="n">
         <v>7</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="D12" s="17" t="n">
+        <v>78</v>
+      </c>
+      <c r="D12" s="18" t="n">
         <v>10071</v>
       </c>
-      <c r="E12" s="18" t="n">
+      <c r="E12" s="19" t="n">
         <v>41526</v>
       </c>
-      <c r="F12" s="17" t="n">
+      <c r="F12" s="18" t="n">
         <v>10463</v>
       </c>
       <c r="G12" s="11" t="s">
@@ -12460,30 +12503,30 @@
       <c r="I12" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="J12" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="K12" s="19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="13" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J12" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="K12" s="20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="13" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="17" t="n">
+        <v>60</v>
+      </c>
+      <c r="B13" s="18" t="n">
         <v>8</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="D13" s="17" t="n">
+        <v>81</v>
+      </c>
+      <c r="D13" s="18" t="n">
         <v>10073</v>
       </c>
-      <c r="E13" s="18" t="n">
+      <c r="E13" s="19" t="n">
         <v>41523</v>
       </c>
-      <c r="F13" s="17" t="n">
+      <c r="F13" s="18" t="n">
         <v>10467</v>
       </c>
       <c r="G13" s="11" t="s">
@@ -12496,27 +12539,27 @@
         <v>35</v>
       </c>
       <c r="J13" s="11"/>
-      <c r="K13" s="19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="14" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K13" s="20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="17" t="n">
+        <v>60</v>
+      </c>
+      <c r="B14" s="18" t="n">
         <v>9</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="D14" s="17" t="n">
+        <v>83</v>
+      </c>
+      <c r="D14" s="18" t="n">
         <v>10075</v>
       </c>
-      <c r="E14" s="18" t="n">
+      <c r="E14" s="19" t="n">
         <v>41528</v>
       </c>
-      <c r="F14" s="17" t="n">
+      <c r="F14" s="18" t="n">
         <v>6893</v>
       </c>
       <c r="G14" s="11" t="s">
@@ -12529,27 +12572,27 @@
         <v>35</v>
       </c>
       <c r="J14" s="11"/>
-      <c r="K14" s="19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="15" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K14" s="20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" s="20" t="n">
+        <v>60</v>
+      </c>
+      <c r="B15" s="21" t="n">
         <v>10</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="D15" s="20" t="n">
+        <v>78</v>
+      </c>
+      <c r="D15" s="21" t="n">
         <v>10079</v>
       </c>
-      <c r="E15" s="21" t="n">
+      <c r="E15" s="22" t="n">
         <v>41529</v>
       </c>
-      <c r="F15" s="20" t="n">
+      <c r="F15" s="21" t="n">
         <v>5874</v>
       </c>
       <c r="G15" s="11" t="s">
@@ -12562,27 +12605,27 @@
         <v>37</v>
       </c>
       <c r="J15" s="11"/>
-      <c r="K15" s="19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="16" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K15" s="20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="16" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="17" t="n">
+        <v>60</v>
+      </c>
+      <c r="B16" s="18" t="n">
         <v>11</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="D16" s="17" t="n">
+        <v>81</v>
+      </c>
+      <c r="D16" s="18" t="n">
         <v>10080</v>
       </c>
-      <c r="E16" s="18" t="n">
+      <c r="E16" s="19" t="n">
         <v>41533</v>
       </c>
-      <c r="F16" s="17"/>
+      <c r="F16" s="18"/>
       <c r="G16" s="11" t="s">
         <v>36</v>
       </c>
@@ -12593,27 +12636,27 @@
         <v>37</v>
       </c>
       <c r="J16" s="11"/>
-      <c r="K16" s="19" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="17" s="19" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K16" s="20" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="17" s="20" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" s="17" t="n">
+        <v>60</v>
+      </c>
+      <c r="B17" s="18" t="n">
         <v>12</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="17" t="n">
+        <v>78</v>
+      </c>
+      <c r="D17" s="18" t="n">
         <v>10081</v>
       </c>
-      <c r="E17" s="18" t="n">
+      <c r="E17" s="19" t="n">
         <v>41531</v>
       </c>
-      <c r="F17" s="17" t="n">
+      <c r="F17" s="18" t="n">
         <v>2235</v>
       </c>
       <c r="G17" s="11" t="s">
@@ -12626,8 +12669,8 @@
         <v>37</v>
       </c>
       <c r="J17" s="11"/>
-      <c r="K17" s="19" t="s">
-        <v>102</v>
+      <c r="K17" s="20" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -12648,17 +12691,17 @@
   </sheetPr>
   <dimension ref="1:198"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.3877551020408"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.8673469387755"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="17.280612244898"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.6326530612245"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="15.3877551020408"/>
@@ -12668,37 +12711,44 @@
     <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
-    <row r="1" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+    <row r="1" s="15" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
       <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H2" s="11" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>106</v>
+        <v>110</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="H3" s="11" t="s">
         <v>16</v>
@@ -12730,25 +12780,25 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>109</v>
+        <v>113</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="H4" s="11" t="s">
         <v>19</v>
@@ -12778,21 +12828,21 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" s="23" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22" t="s">
-        <v>110</v>
-      </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
+    <row r="5" s="24" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="23"/>
+      <c r="B5" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="23"/>
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
       <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>133</v>
@@ -12801,15 +12851,15 @@
         <v>10.36813775</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="G6" s="24" t="n">
+        <v>92</v>
+      </c>
+      <c r="G6" s="25" t="n">
         <v>41585</v>
       </c>
       <c r="H6" s="11" t="s">
@@ -12824,7 +12874,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>133</v>
@@ -12833,15 +12883,15 @@
         <v>3.459</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="G7" s="24" t="n">
+        <v>92</v>
+      </c>
+      <c r="G7" s="25" t="n">
         <v>41585</v>
       </c>
       <c r="H7" s="11" t="s">
@@ -12856,7 +12906,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>133</v>
@@ -12865,15 +12915,15 @@
         <v>6.01</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="G8" s="24" t="n">
+        <v>92</v>
+      </c>
+      <c r="G8" s="25" t="n">
         <v>41585</v>
       </c>
       <c r="H8" s="11" t="s">
@@ -12888,7 +12938,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>133</v>
@@ -12897,15 +12947,15 @@
         <v>10.777</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="G9" s="24" t="n">
+        <v>92</v>
+      </c>
+      <c r="G9" s="25" t="n">
         <v>41585</v>
       </c>
       <c r="H9" s="11" t="s">
@@ -12920,7 +12970,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>133</v>
@@ -12929,19 +12979,19 @@
         <v>12.241</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="G10" s="24" t="n">
+        <v>92</v>
+      </c>
+      <c r="G10" s="25" t="n">
         <v>41585</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="I10" s="11" t="s">
         <v>22</v>
@@ -12950,19 +13000,19 @@
       <c r="AMH10" s="0"/>
       <c r="AMI10" s="0"/>
     </row>
-    <row r="11" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="25"/>
-      <c r="B11" s="25" t="s">
-        <v>112</v>
-      </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="26"/>
-      <c r="AMG11" s="25"/>
-      <c r="AMH11" s="25"/>
-      <c r="AMI11" s="25"/>
+    <row r="11" s="28" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="26"/>
+      <c r="B11" s="26" t="s">
+        <v>116</v>
+      </c>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="26"/>
+      <c r="F11" s="26"/>
+      <c r="G11" s="27"/>
+      <c r="AMG11" s="26"/>
+      <c r="AMH11" s="26"/>
+      <c r="AMI11" s="26"/>
       <c r="AMJ11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12976,15 +13026,15 @@
         <v>-0.239</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F12" s="0" t="n">
         <v>0.544289172561245</v>
       </c>
-      <c r="G12" s="24" t="n">
+      <c r="G12" s="25" t="n">
         <v>33688.0010367361</v>
       </c>
       <c r="AMG12" s="0"/>
@@ -13002,15 +13052,15 @@
         <v>-0.235</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F13" s="0" t="n">
         <v>0.342962256667443</v>
       </c>
-      <c r="G13" s="24" t="n">
+      <c r="G13" s="25" t="n">
         <v>33688.0010367477</v>
       </c>
       <c r="AMG13" s="0"/>
@@ -13028,15 +13078,15 @@
         <v>-0.234</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F14" s="0" t="n">
         <v>0.705070090605723</v>
       </c>
-      <c r="G14" s="24" t="n">
+      <c r="G14" s="25" t="n">
         <v>33688.0010367593</v>
       </c>
       <c r="AMG14" s="0"/>
@@ -13054,15 +13104,15 @@
         <v>-0.2505</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>0.419306807938575</v>
       </c>
-      <c r="G15" s="24" t="n">
+      <c r="G15" s="25" t="n">
         <v>33688.0010367708</v>
       </c>
       <c r="AMG15" s="0"/>
@@ -13080,39 +13130,39 @@
         <v>-0.2355</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="F16" s="0" t="n">
         <v>0.378187846455892</v>
       </c>
-      <c r="G16" s="24" t="n">
+      <c r="G16" s="25" t="n">
         <v>33688.0010367824</v>
       </c>
       <c r="AMG16" s="0"/>
       <c r="AMH16" s="0"/>
       <c r="AMI16" s="0"/>
     </row>
-    <row r="17" s="30" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="28"/>
-      <c r="B17" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-      <c r="G17" s="29"/>
-      <c r="AMG17" s="28"/>
-      <c r="AMH17" s="28"/>
-      <c r="AMI17" s="28"/>
+    <row r="17" s="31" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="29"/>
+      <c r="B17" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="30"/>
+      <c r="AMG17" s="29"/>
+      <c r="AMH17" s="29"/>
+      <c r="AMI17" s="29"/>
       <c r="AMJ17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>2740</v>
@@ -13129,7 +13179,7 @@
       <c r="F18" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="G18" s="24" t="n">
+      <c r="G18" s="25" t="n">
         <v>41561</v>
       </c>
       <c r="H18" s="11" t="s">
@@ -13144,7 +13194,7 @@
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>3724</v>
@@ -13161,7 +13211,7 @@
       <c r="F19" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="G19" s="24" t="n">
+      <c r="G19" s="25" t="n">
         <v>41583</v>
       </c>
       <c r="H19" s="11" t="s">
@@ -13176,7 +13226,7 @@
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>2793</v>
@@ -13193,7 +13243,7 @@
       <c r="F20" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="G20" s="24" t="n">
+      <c r="G20" s="25" t="n">
         <v>41595</v>
       </c>
       <c r="H20" s="11" t="s">
@@ -13208,7 +13258,7 @@
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>3615</v>
@@ -13225,7 +13275,7 @@
       <c r="F21" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="G21" s="24" t="n">
+      <c r="G21" s="25" t="n">
         <v>41621</v>
       </c>
       <c r="H21" s="11" t="s">
@@ -13240,7 +13290,7 @@
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>745</v>
@@ -13257,11 +13307,11 @@
       <c r="F22" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="G22" s="24" t="n">
+      <c r="G22" s="25" t="n">
         <v>41535</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>111</v>
+        <v>115</v>
       </c>
       <c r="I22" s="11" t="s">
         <v>22</v>
@@ -13271,442 +13321,442 @@
       <c r="AMI22" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D53" s="31"/>
+      <c r="D53" s="32"/>
     </row>
     <row r="54" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D54" s="31"/>
+      <c r="D54" s="32"/>
     </row>
     <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D55" s="31"/>
+      <c r="D55" s="32"/>
     </row>
     <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D56" s="31"/>
+      <c r="D56" s="32"/>
     </row>
     <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D57" s="31"/>
+      <c r="D57" s="32"/>
     </row>
     <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D58" s="31"/>
+      <c r="D58" s="32"/>
     </row>
     <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D59" s="31"/>
+      <c r="D59" s="32"/>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D60" s="31"/>
+      <c r="D60" s="32"/>
     </row>
     <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D61" s="31"/>
+      <c r="D61" s="32"/>
     </row>
     <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D62" s="31"/>
+      <c r="D62" s="32"/>
     </row>
     <row r="63" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D63" s="31"/>
+      <c r="D63" s="32"/>
     </row>
     <row r="64" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D64" s="31"/>
+      <c r="D64" s="32"/>
     </row>
     <row r="65" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D65" s="31"/>
+      <c r="D65" s="32"/>
     </row>
     <row r="66" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D66" s="31"/>
+      <c r="D66" s="32"/>
     </row>
     <row r="67" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D67" s="31"/>
+      <c r="D67" s="32"/>
     </row>
     <row r="68" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D68" s="31"/>
+      <c r="D68" s="32"/>
     </row>
     <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D69" s="31"/>
+      <c r="D69" s="32"/>
     </row>
     <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D70" s="31"/>
+      <c r="D70" s="32"/>
     </row>
     <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D71" s="31"/>
+      <c r="D71" s="32"/>
     </row>
     <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D72" s="31"/>
+      <c r="D72" s="32"/>
     </row>
     <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D73" s="31"/>
+      <c r="D73" s="32"/>
     </row>
     <row r="74" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D74" s="31"/>
+      <c r="D74" s="32"/>
     </row>
     <row r="75" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D75" s="31"/>
+      <c r="D75" s="32"/>
     </row>
     <row r="76" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D76" s="31"/>
+      <c r="D76" s="32"/>
     </row>
     <row r="77" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D77" s="31"/>
+      <c r="D77" s="32"/>
     </row>
     <row r="78" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D78" s="31"/>
+      <c r="D78" s="32"/>
     </row>
     <row r="79" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D79" s="31"/>
+      <c r="D79" s="32"/>
     </row>
     <row r="80" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D80" s="31"/>
+      <c r="D80" s="32"/>
     </row>
     <row r="81" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D81" s="31"/>
+      <c r="D81" s="32"/>
     </row>
     <row r="82" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D82" s="31"/>
+      <c r="D82" s="32"/>
     </row>
     <row r="83" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D83" s="31"/>
+      <c r="D83" s="32"/>
     </row>
     <row r="84" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D84" s="31"/>
+      <c r="D84" s="32"/>
     </row>
     <row r="85" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D85" s="31"/>
+      <c r="D85" s="32"/>
     </row>
     <row r="86" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D86" s="31"/>
+      <c r="D86" s="32"/>
     </row>
     <row r="87" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D87" s="32"/>
+      <c r="D87" s="33"/>
     </row>
     <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D88" s="32"/>
+      <c r="D88" s="33"/>
     </row>
     <row r="89" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D89" s="32"/>
+      <c r="D89" s="33"/>
     </row>
     <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D90" s="32"/>
+      <c r="D90" s="33"/>
     </row>
     <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D91" s="32"/>
+      <c r="D91" s="33"/>
     </row>
     <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D92" s="32"/>
+      <c r="D92" s="33"/>
     </row>
     <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D93" s="32"/>
+      <c r="D93" s="33"/>
     </row>
     <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D94" s="32"/>
+      <c r="D94" s="33"/>
     </row>
     <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D95" s="32"/>
+      <c r="D95" s="33"/>
     </row>
     <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D96" s="32"/>
+      <c r="D96" s="33"/>
     </row>
     <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D97" s="32"/>
+      <c r="D97" s="33"/>
     </row>
     <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D98" s="32"/>
+      <c r="D98" s="33"/>
     </row>
     <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D99" s="32"/>
+      <c r="D99" s="33"/>
     </row>
     <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D100" s="32"/>
+      <c r="D100" s="33"/>
     </row>
     <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D101" s="32"/>
+      <c r="D101" s="33"/>
     </row>
     <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D102" s="32"/>
+      <c r="D102" s="33"/>
     </row>
     <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D103" s="32"/>
+      <c r="D103" s="33"/>
     </row>
     <row r="104" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D104" s="32"/>
+      <c r="D104" s="33"/>
     </row>
     <row r="105" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D105" s="32"/>
+      <c r="D105" s="33"/>
     </row>
     <row r="106" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D106" s="32"/>
+      <c r="D106" s="33"/>
     </row>
     <row r="107" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D107" s="32"/>
+      <c r="D107" s="33"/>
     </row>
     <row r="108" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D108" s="32"/>
+      <c r="D108" s="33"/>
     </row>
     <row r="109" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D109" s="32"/>
+      <c r="D109" s="33"/>
     </row>
     <row r="110" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D110" s="32"/>
+      <c r="D110" s="33"/>
     </row>
     <row r="111" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D111" s="32"/>
+      <c r="D111" s="33"/>
     </row>
     <row r="112" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D112" s="32"/>
+      <c r="D112" s="33"/>
     </row>
     <row r="113" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D113" s="32"/>
+      <c r="D113" s="33"/>
     </row>
     <row r="114" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D114" s="32"/>
+      <c r="D114" s="33"/>
     </row>
     <row r="115" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D115" s="32"/>
+      <c r="D115" s="33"/>
     </row>
     <row r="116" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D116" s="32"/>
+      <c r="D116" s="33"/>
     </row>
     <row r="117" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D117" s="32"/>
+      <c r="D117" s="33"/>
     </row>
     <row r="118" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D118" s="32"/>
+      <c r="D118" s="33"/>
     </row>
     <row r="119" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D119" s="32"/>
+      <c r="D119" s="33"/>
     </row>
     <row r="120" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D120" s="32"/>
+      <c r="D120" s="33"/>
     </row>
     <row r="121" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D121" s="31"/>
+      <c r="D121" s="32"/>
     </row>
     <row r="122" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D122" s="31"/>
+      <c r="D122" s="32"/>
     </row>
     <row r="123" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D123" s="31"/>
+      <c r="D123" s="32"/>
     </row>
     <row r="124" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D124" s="31"/>
+      <c r="D124" s="32"/>
     </row>
     <row r="125" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D125" s="31"/>
+      <c r="D125" s="32"/>
     </row>
     <row r="126" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D126" s="31"/>
+      <c r="D126" s="32"/>
     </row>
     <row r="127" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D127" s="31"/>
+      <c r="D127" s="32"/>
     </row>
     <row r="128" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D128" s="31"/>
+      <c r="D128" s="32"/>
     </row>
     <row r="129" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D129" s="31"/>
+      <c r="D129" s="32"/>
     </row>
     <row r="130" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D130" s="31"/>
+      <c r="D130" s="32"/>
     </row>
     <row r="131" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D131" s="31"/>
+      <c r="D131" s="32"/>
     </row>
     <row r="132" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D132" s="31"/>
+      <c r="D132" s="32"/>
     </row>
     <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D133" s="31"/>
+      <c r="D133" s="32"/>
     </row>
     <row r="134" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D134" s="31"/>
+      <c r="D134" s="32"/>
     </row>
     <row r="135" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D135" s="31"/>
+      <c r="D135" s="32"/>
     </row>
     <row r="136" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D136" s="31"/>
+      <c r="D136" s="32"/>
     </row>
     <row r="137" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D137" s="31"/>
+      <c r="D137" s="32"/>
     </row>
     <row r="138" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D138" s="31"/>
+      <c r="D138" s="32"/>
     </row>
     <row r="139" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D139" s="31"/>
+      <c r="D139" s="32"/>
     </row>
     <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D140" s="31"/>
+      <c r="D140" s="32"/>
     </row>
     <row r="141" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D141" s="31"/>
+      <c r="D141" s="32"/>
     </row>
     <row r="142" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D142" s="31"/>
+      <c r="D142" s="32"/>
     </row>
     <row r="143" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D143" s="31"/>
+      <c r="D143" s="32"/>
     </row>
     <row r="144" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D144" s="31"/>
+      <c r="D144" s="32"/>
     </row>
     <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D145" s="31"/>
+      <c r="D145" s="32"/>
     </row>
     <row r="146" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D146" s="31"/>
+      <c r="D146" s="32"/>
     </row>
     <row r="147" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D147" s="31"/>
+      <c r="D147" s="32"/>
     </row>
     <row r="148" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D148" s="31"/>
+      <c r="D148" s="32"/>
     </row>
     <row r="149" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D149" s="31"/>
+      <c r="D149" s="32"/>
     </row>
     <row r="150" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D150" s="31"/>
+      <c r="D150" s="32"/>
     </row>
     <row r="151" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D151" s="31"/>
+      <c r="D151" s="32"/>
     </row>
     <row r="152" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D152" s="31"/>
+      <c r="D152" s="32"/>
     </row>
     <row r="153" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D153" s="31"/>
+      <c r="D153" s="32"/>
     </row>
     <row r="154" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D154" s="31"/>
+      <c r="D154" s="32"/>
     </row>
     <row r="155" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D155" s="31"/>
+      <c r="D155" s="32"/>
     </row>
     <row r="156" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D156" s="31"/>
+      <c r="D156" s="32"/>
     </row>
     <row r="157" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D157" s="32"/>
+      <c r="D157" s="33"/>
     </row>
     <row r="158" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D158" s="32"/>
+      <c r="D158" s="33"/>
     </row>
     <row r="159" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D159" s="32"/>
+      <c r="D159" s="33"/>
     </row>
     <row r="160" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D160" s="32"/>
+      <c r="D160" s="33"/>
     </row>
     <row r="161" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D161" s="32"/>
+      <c r="D161" s="33"/>
     </row>
     <row r="162" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D162" s="32"/>
+      <c r="D162" s="33"/>
     </row>
     <row r="163" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D163" s="32"/>
+      <c r="D163" s="33"/>
     </row>
     <row r="164" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D164" s="32"/>
+      <c r="D164" s="33"/>
     </row>
     <row r="165" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D165" s="32"/>
+      <c r="D165" s="33"/>
     </row>
     <row r="166" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D166" s="32"/>
+      <c r="D166" s="33"/>
     </row>
     <row r="167" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D167" s="32"/>
+      <c r="D167" s="33"/>
     </row>
     <row r="168" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D168" s="32"/>
+      <c r="D168" s="33"/>
     </row>
     <row r="169" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D169" s="32"/>
+      <c r="D169" s="33"/>
     </row>
     <row r="170" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D170" s="32"/>
+      <c r="D170" s="33"/>
     </row>
     <row r="171" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D171" s="32"/>
+      <c r="D171" s="33"/>
     </row>
     <row r="172" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D172" s="32"/>
+      <c r="D172" s="33"/>
     </row>
     <row r="173" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D173" s="32"/>
+      <c r="D173" s="33"/>
     </row>
     <row r="174" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D174" s="32"/>
+      <c r="D174" s="33"/>
     </row>
     <row r="175" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D175" s="32"/>
+      <c r="D175" s="33"/>
     </row>
     <row r="176" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D176" s="32"/>
+      <c r="D176" s="33"/>
     </row>
     <row r="177" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D177" s="32"/>
+      <c r="D177" s="33"/>
     </row>
     <row r="178" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D178" s="31"/>
+      <c r="D178" s="32"/>
     </row>
     <row r="179" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D179" s="31"/>
+      <c r="D179" s="32"/>
     </row>
     <row r="180" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D180" s="31"/>
+      <c r="D180" s="32"/>
     </row>
     <row r="181" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D181" s="31"/>
+      <c r="D181" s="32"/>
     </row>
     <row r="182" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D182" s="31"/>
+      <c r="D182" s="32"/>
     </row>
     <row r="183" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D183" s="31"/>
+      <c r="D183" s="32"/>
     </row>
     <row r="184" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D184" s="31"/>
+      <c r="D184" s="32"/>
     </row>
     <row r="185" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D185" s="31"/>
+      <c r="D185" s="32"/>
     </row>
     <row r="186" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D186" s="31"/>
+      <c r="D186" s="32"/>
     </row>
     <row r="187" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D187" s="31"/>
+      <c r="D187" s="32"/>
     </row>
     <row r="188" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D188" s="31"/>
+      <c r="D188" s="32"/>
     </row>
     <row r="189" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D189" s="31"/>
+      <c r="D189" s="32"/>
     </row>
     <row r="190" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D190" s="31"/>
+      <c r="D190" s="32"/>
     </row>
     <row r="191" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D191" s="31"/>
+      <c r="D191" s="32"/>
     </row>
     <row r="192" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D192" s="31"/>
+      <c r="D192" s="32"/>
     </row>
     <row r="193" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D193" s="31"/>
+      <c r="D193" s="32"/>
     </row>
     <row r="194" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D194" s="31"/>
+      <c r="D194" s="32"/>
     </row>
     <row r="195" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D195" s="31"/>
+      <c r="D195" s="32"/>
     </row>
     <row r="196" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D196" s="31"/>
+      <c r="D196" s="32"/>
     </row>
     <row r="197" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D197" s="31"/>
+      <c r="D197" s="32"/>
     </row>
     <row r="198" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D198" s="31"/>
+      <c r="D198" s="32"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -13741,7 +13791,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B1" s="0" t="s">
         <v>16</v>
@@ -13755,7 +13805,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B2" s="0" t="s">
         <v>19</v>
@@ -13907,7 +13957,7 @@
       <c r="A18" s="0" t="n">
         <v>22606</v>
       </c>
-      <c r="B18" s="33" t="n">
+      <c r="B18" s="34" t="n">
         <v>33137</v>
       </c>
       <c r="C18" s="0" t="s">
@@ -13918,7 +13968,7 @@
       <c r="A19" s="0" t="n">
         <v>22607</v>
       </c>
-      <c r="B19" s="33" t="n">
+      <c r="B19" s="34" t="n">
         <v>33368</v>
       </c>
       <c r="C19" s="0" t="s">

</xml_diff>